<commit_message>
Fixed mistake in power tree
</commit_message>
<xml_diff>
--- a/Power tree.xlsx
+++ b/Power tree.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heinecke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Downloads\SBC5-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CCA29E-2409-405A-A194-00131A3DC3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED0A87D-05D2-40DD-A8FE-B007201A38E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{E72A3546-5772-4171-86E1-18A31D0176B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{E72A3546-5772-4171-86E1-18A31D0176B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Buck converters" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -703,7 +703,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -734,44 +734,17 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -790,7 +763,37 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,13 +801,13 @@
   </cellStyles>
   <dxfs count="62">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
       <font>
@@ -828,34 +831,42 @@
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -879,50 +890,16 @@
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -943,17 +920,214 @@
       </font>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -977,193 +1151,22 @@
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1179,32 +1182,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{92E29884-83E4-4CB9-941E-86581A7C7D24}" name="Table9" displayName="Table9" ref="B1:L3" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{92E29884-83E4-4CB9-941E-86581A7C7D24}" name="Table9" displayName="Table9" ref="B1:L3" totalsRowShown="0" headerRowDxfId="61">
   <autoFilter ref="B1:L3" xr:uid="{8837DF0B-F947-47F6-BAB2-639251F47D32}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{64AF6BF8-06D8-456B-B292-58F47ECF9BF9}" name="Input voltage_x000a_(V)"/>
-    <tableColumn id="2" xr3:uid="{875EC177-152A-4041-9ECC-8D9CABF22856}" name="Current in_x000a_(mA)" dataDxfId="21">
+    <tableColumn id="2" xr3:uid="{875EC177-152A-4041-9ECC-8D9CABF22856}" name="Current in_x000a_(mA)" dataDxfId="60">
       <calculatedColumnFormula>I2/B2/L2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C290F034-A301-4C58-9CBE-BBFFA79FEBF9}" name="Power in_x000a_(mW)" dataDxfId="20">
+    <tableColumn id="3" xr3:uid="{C290F034-A301-4C58-9CBE-BBFFA79FEBF9}" name="Power in_x000a_(mW)" dataDxfId="59">
       <calculatedColumnFormula>B2*C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{215BC251-9678-4D00-A85C-B906B9DF625D}" name="Power in_x000a_(W)" dataDxfId="19">
+    <tableColumn id="4" xr3:uid="{215BC251-9678-4D00-A85C-B906B9DF625D}" name="Power in_x000a_(W)" dataDxfId="58">
       <calculatedColumnFormula>D2/1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{1C531A31-A671-4CEA-98D0-048400BE54C9}" name="Sink"/>
     <tableColumn id="6" xr3:uid="{A7C731B7-F2F9-4285-B64D-072DE649CF9E}" name="Output voltage_x000a_(V)"/>
     <tableColumn id="7" xr3:uid="{FB4AAEE5-7DF8-4806-866E-FF20D7AFDFBC}" name="Current out_x000a_(mA)"/>
-    <tableColumn id="8" xr3:uid="{648F6602-28B0-4537-AE22-5CC1B9E6F90C}" name="Power out_x000a_(mW)" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{648F6602-28B0-4537-AE22-5CC1B9E6F90C}" name="Power out_x000a_(mW)" dataDxfId="57">
       <calculatedColumnFormula>G2*H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{460B383B-76D0-4DB4-9FCE-9AF75B108791}" name="Power out_x000a_(W)" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{460B383B-76D0-4DB4-9FCE-9AF75B108791}" name="Power out_x000a_(W)" dataDxfId="56">
       <calculatedColumnFormula>I2/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{1B8CC755-9B2B-49E4-8D96-E8F4ED827615}" name="Heat loss_x000a_(W)" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{1B8CC755-9B2B-49E4-8D96-E8F4ED827615}" name="Heat loss_x000a_(W)" dataDxfId="55">
       <calculatedColumnFormula>E2-J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{8DA88ED1-BA42-4B1B-9AC4-C6709E7CC53A}" name="Efficiency" dataDxfId="15" dataCellStyle="Percent"/>
+    <tableColumn id="11" xr3:uid="{8DA88ED1-BA42-4B1B-9AC4-C6709E7CC53A}" name="Efficiency" dataDxfId="54" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1236,7 +1239,7 @@
   <autoFilter ref="B7:F9" xr:uid="{B590B994-F24D-43D5-AAE1-AB5C0F39A5D2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3D41CA9D-FB20-4377-96AD-31856310779A}" name="Sink"/>
-    <tableColumn id="2" xr3:uid="{ECD64578-F73E-4642-8F0B-D740A4556471}" name="Voltage (V)" dataDxfId="26">
+    <tableColumn id="2" xr3:uid="{ECD64578-F73E-4642-8F0B-D740A4556471}" name="Voltage (V)" dataDxfId="0">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{E99D08CC-593B-447B-BB41-7CEC089F938A}" name="Current (mA)">
@@ -1254,7 +1257,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{728C2D89-6433-4009-ABEA-301F2EE0BDA6}" name="Table10" displayName="Table10" ref="B1:T14" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{728C2D89-6433-4009-ABEA-301F2EE0BDA6}" name="Table10" displayName="Table10" ref="B1:T14" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="B1:T14" xr:uid="{660142C1-230E-4338-B7F9-2B1ABCB59A99}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{C32C9119-92FB-4C2B-B78D-96AA99DBA12F}" name="Source"/>
@@ -1264,32 +1267,32 @@
     <tableColumn id="5" xr3:uid="{317C6DA6-006D-4E68-87A7-44DCA77A817B}" name="Current in (mA)">
       <calculatedColumnFormula>O2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FE486BB4-7D80-47E4-B777-07DDD266AECC}" name="Power in (mW)" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{FE486BB4-7D80-47E4-B777-07DDD266AECC}" name="Power in (mW)" dataDxfId="26">
       <calculatedColumnFormula>E2*F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0133FC51-05E5-4966-8DCD-0A90CF67BB88}" name="Power in (W)" dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{0133FC51-05E5-4966-8DCD-0A90CF67BB88}" name="Power in (W)" dataDxfId="25">
       <calculatedColumnFormula>G2/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{1C09D616-C725-4140-B7DE-6B6580E5CD8C}" name="Max current out (mA)" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{9D26CC57-EE4B-4296-B55A-0316411A369B}" name="Output" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{1C09D616-C725-4140-B7DE-6B6580E5CD8C}" name="Max current out (mA)" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{9D26CC57-EE4B-4296-B55A-0316411A369B}" name="Output" dataDxfId="23"/>
     <tableColumn id="10" xr3:uid="{B957A170-8C95-4B29-B00B-C973C936787E}" name="Sink"/>
     <tableColumn id="11" xr3:uid="{EE32E27A-BD83-4BCA-8589-554F25AC8715}" name="Min voltage out (V)"/>
     <tableColumn id="12" xr3:uid="{3AF01889-8D2D-4EAC-97B9-547901DCCAFE}" name="Max voltage out (V)"/>
     <tableColumn id="13" xr3:uid="{173A4E0F-633C-4FF3-B73F-718616C6BC8F}" name="Voltage out (V)"/>
-    <tableColumn id="14" xr3:uid="{5E1BB9C2-59E5-4565-AEF8-6C592777FF6B}" name="Current out (mA)" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{DC560683-4A87-4E70-8DC8-8096A3C362C3}" name="Power out (mW)" dataDxfId="6">
+    <tableColumn id="14" xr3:uid="{5E1BB9C2-59E5-4565-AEF8-6C592777FF6B}" name="Current out (mA)" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{DC560683-4A87-4E70-8DC8-8096A3C362C3}" name="Power out (mW)" dataDxfId="21">
       <calculatedColumnFormula>N2*O2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{855B29C6-554F-46B9-94DB-149D10271BD4}" name="Power out (W)" dataDxfId="5">
+    <tableColumn id="16" xr3:uid="{855B29C6-554F-46B9-94DB-149D10271BD4}" name="Power out (W)" dataDxfId="20">
       <calculatedColumnFormula>P2/1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="17" xr3:uid="{6FBB9F3C-240D-4933-9B15-D15CD70B30DB}" name="Voltage drop (V)">
       <calculatedColumnFormula>E2-N2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{D283933F-6F5F-4BA8-9367-4D75B51F4D5D}" name="Heat loss (W)" dataDxfId="4">
+    <tableColumn id="18" xr3:uid="{D283933F-6F5F-4BA8-9367-4D75B51F4D5D}" name="Heat loss (W)" dataDxfId="19">
       <calculatedColumnFormula>H2-Q2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{02EC7941-E4D9-4CDB-97EC-81FDC39262D7}" name="Efficiency" dataDxfId="3" dataCellStyle="Percent">
+    <tableColumn id="19" xr3:uid="{02EC7941-E4D9-4CDB-97EC-81FDC39262D7}" name="Efficiency" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(H2=0,1,Q2/H2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1298,7 +1301,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7F86B533-7364-4BB7-AAAA-D8DEE6FBB573}" name="Table11" displayName="Table11" ref="B18:H23" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7F86B533-7364-4BB7-AAAA-D8DEE6FBB573}" name="Table11" displayName="Table11" ref="B18:H23" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="B18:H23" xr:uid="{DB6740D6-ABDF-4DE8-998E-29F3E18761F9}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2D34AD4E-9D3F-49AA-ABF6-FEFD15E0CF5F}" name="Source"/>
@@ -1306,10 +1309,10 @@
     <tableColumn id="3" xr3:uid="{7AB22D95-8FD0-4E90-A14A-CC6508DC5FDD}" name="Max voltage in (V)"/>
     <tableColumn id="4" xr3:uid="{1169AF06-C16B-4030-942F-D01A16E4157B}" name="Voltage in (V)"/>
     <tableColumn id="5" xr3:uid="{F5AB428D-CAB8-494D-9165-72BB2FBF89CB}" name="Current in (mA)"/>
-    <tableColumn id="6" xr3:uid="{E63A8BCE-0EE7-4654-B919-65E9385046AB}" name="Power in (mW)" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{E63A8BCE-0EE7-4654-B919-65E9385046AB}" name="Power in (mW)" dataDxfId="16">
       <calculatedColumnFormula>E19*F19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DE9D0662-A10B-4C04-A663-1C90DCA5B981}" name="Power in (W)" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{DE9D0662-A10B-4C04-A663-1C90DCA5B981}" name="Power in (W)" dataDxfId="15">
       <calculatedColumnFormula>G19/1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1318,7 +1321,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{559CCFC3-5F07-45CA-9386-336DA9DCEC0D}" name="Table12" displayName="Table12" ref="K18:O21" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{559CCFC3-5F07-45CA-9386-336DA9DCEC0D}" name="Table12" displayName="Table12" ref="K18:O21" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="K18:O21" xr:uid="{C020B84F-A046-4B5B-B5F1-18402570AC4C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9DC3A4C0-E85B-48A0-AEE7-6AAA4C8B63C0}" name="Sinks"/>
@@ -1327,7 +1330,7 @@
     <tableColumn id="4" xr3:uid="{31999E69-D6D9-46B0-BFFB-EFB189C1EAB6}" name="Power in (mW)">
       <calculatedColumnFormula>L19*M19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9C3C5FE4-08C2-4E0C-8305-98BC461454F5}" name="Power in (W)" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{9C3C5FE4-08C2-4E0C-8305-98BC461454F5}" name="Power in (W)" dataDxfId="13">
       <calculatedColumnFormula>N19/1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1336,16 +1339,16 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1114EC46-03A0-4ED4-9517-32D73F2DBAFD}" name="Table5" displayName="Table5" ref="B1:F2" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1114EC46-03A0-4ED4-9517-32D73F2DBAFD}" name="Table5" displayName="Table5" ref="B1:F2" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="B1:F2" xr:uid="{3A6101FE-8D0D-4071-A18D-7C3560B79C30}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{72E3BD3C-CA2B-4657-A05C-D072C6C7961C}" name="Sink" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{72E3BD3C-CA2B-4657-A05C-D072C6C7961C}" name="Sink" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{570C98D0-73CD-4B61-B4B6-B3C077CEA15C}" name="Voltage (V)"/>
     <tableColumn id="3" xr3:uid="{B4FD65A7-DDF3-44D8-81EC-C1A94FEA0D8E}" name="Current (mA)"/>
-    <tableColumn id="4" xr3:uid="{F8A0947B-24CF-4BB9-AA30-CC6EDBB5E178}" name="Power (mW)" dataDxfId="24">
+    <tableColumn id="4" xr3:uid="{F8A0947B-24CF-4BB9-AA30-CC6EDBB5E178}" name="Power (mW)" dataDxfId="8">
       <calculatedColumnFormula>D2*C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BD83BC3A-DAAD-4274-832F-3FD01B430CA6}" name="Power (W)" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{BD83BC3A-DAAD-4274-832F-3FD01B430CA6}" name="Power (W)" dataDxfId="7">
       <calculatedColumnFormula>E2/1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1361,7 +1364,7 @@
     <tableColumn id="2" xr3:uid="{F50F894B-AB63-4B3A-A49A-F65D5ABB32D9}" name="Voltage (V)"/>
     <tableColumn id="3" xr3:uid="{73310900-DEBA-4348-8E3A-39A10BBA45AA}" name="Current (mA)"/>
     <tableColumn id="4" xr3:uid="{008C10E9-8D15-4037-8C66-5232AD8F1671}" name="Power (mW)"/>
-    <tableColumn id="5" xr3:uid="{DD05115D-C945-4C00-AABD-0E5D5C38B729}" name="Power (W)" dataDxfId="35">
+    <tableColumn id="5" xr3:uid="{DD05115D-C945-4C00-AABD-0E5D5C38B729}" name="Power (W)" dataDxfId="6">
       <calculatedColumnFormula>E2/1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1376,10 +1379,10 @@
     <tableColumn id="1" xr3:uid="{C2B77D68-610C-45C2-A1E7-DADE40229038}" name="Sink"/>
     <tableColumn id="2" xr3:uid="{B2A67EEF-BED3-40E4-A057-6360AC85B1D4}" name="Voltage (V)"/>
     <tableColumn id="3" xr3:uid="{E54580B1-0317-42DA-AAAC-8A874DFF8997}" name="Current (mA)"/>
-    <tableColumn id="4" xr3:uid="{51960A38-2E5D-4C0C-815F-860C62579BFD}" name="Power (mW)" dataDxfId="34">
+    <tableColumn id="4" xr3:uid="{51960A38-2E5D-4C0C-815F-860C62579BFD}" name="Power (mW)" dataDxfId="5">
       <calculatedColumnFormula>C21*D21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{26AC31C2-EB8A-40E3-9D81-D5CCCFB3A51E}" name="Power (W)" dataDxfId="33">
+    <tableColumn id="5" xr3:uid="{26AC31C2-EB8A-40E3-9D81-D5CCCFB3A51E}" name="Power (W)" dataDxfId="4">
       <calculatedColumnFormula>E21/1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1404,7 +1407,7 @@
     <tableColumn id="7" xr3:uid="{6CBD30A4-777A-4B77-BCC3-AA2D89C0E42C}" name="LDO power lost (W)">
       <calculatedColumnFormula>(K2-J2)*L2/1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{623667BF-2457-4802-B8CD-2579388158E0}" name="Efficiency" dataDxfId="32" dataCellStyle="Percent">
+    <tableColumn id="8" xr3:uid="{623667BF-2457-4802-B8CD-2579388158E0}" name="Efficiency" dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>(N2-O2)/N2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1419,9 +1422,9 @@
     <tableColumn id="1" xr3:uid="{0655E15C-2445-44F5-8DFB-8932359691AD}" name="Sink"/>
     <tableColumn id="2" xr3:uid="{75AC5B89-4231-41FE-873D-325BA0B5DB7F}" name="Voltage (V)"/>
     <tableColumn id="3" xr3:uid="{C32987F5-324A-4AAB-BC93-AC8BE297E733}" name="Number of pins"/>
-    <tableColumn id="4" xr3:uid="{34192BDA-FC9C-44A3-9D3B-16ABFD0528C4}" name="Capacitance (F)" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{34192BDA-FC9C-44A3-9D3B-16ABFD0528C4}" name="Capacitance (F)" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{3A4A1471-8852-4C33-AB93-9F503D480C58}" name="Frequency (Hz)"/>
-    <tableColumn id="6" xr3:uid="{1E36DBC9-59AA-45A2-9136-FE0DB7C1010C}" name="Current (mA)" dataDxfId="30">
+    <tableColumn id="6" xr3:uid="{1E36DBC9-59AA-45A2-9136-FE0DB7C1010C}" name="Current (mA)" dataDxfId="1">
       <calculatedColumnFormula>1000*K17*L17*J17*0.5*M17</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{B52E8B41-12A9-4440-A949-A9CDEC8E10B8}" name="Power (mW)">
@@ -1734,7 +1737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2968E912-AAF4-43C0-A76F-CA791995FA7C}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -1753,45 +1756,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="42" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
+      <c r="A2" s="48"/>
       <c r="B2" s="8">
         <v>12</v>
       </c>
@@ -1835,7 +1838,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="8">
         <v>12</v>
       </c>
@@ -1877,7 +1880,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1891,38 +1894,38 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="52" t="s">
+      <c r="A5" s="49"/>
+      <c r="B5" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="37">
         <f>SUM(C2:C3)</f>
         <v>1035.399252920696</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="37">
         <f>SUM(D2:D3)</f>
         <v>12424.791035048353</v>
       </c>
-      <c r="E5" s="53">
+      <c r="E5" s="44">
         <f>SUM(E2:E3)</f>
         <v>12.424791035048353</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46">
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="37">
         <f>SUM(I2:I3)</f>
         <v>9808.6948451733333</v>
       </c>
-      <c r="J5" s="53">
+      <c r="J5" s="44">
         <f>SUM(J2:J3)</f>
         <v>9.8086948451733331</v>
       </c>
-      <c r="K5" s="54">
+      <c r="K5" s="45">
         <f>SUM(K2:K3)</f>
         <v>2.6160961898750195</v>
       </c>
-      <c r="L5" s="55">
+      <c r="L5" s="46">
         <f>J5/E5</f>
         <v>0.78944545767446472</v>
       </c>
@@ -1970,70 +1973,70 @@
     <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="N1" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="50" t="s">
+      <c r="O1" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="50" t="s">
+      <c r="P1" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="50" t="s">
+      <c r="Q1" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="42" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
+      <c r="A2" s="51"/>
       <c r="B2" s="8" t="s">
         <v>62</v>
       </c>
@@ -2103,7 +2106,7 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="8" t="s">
         <v>73</v>
       </c>
@@ -2174,7 +2177,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="8" t="s">
         <v>63</v>
       </c>
@@ -2245,7 +2248,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="8" t="s">
         <v>64</v>
       </c>
@@ -2316,7 +2319,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="8" t="s">
         <v>93</v>
       </c>
@@ -2383,7 +2386,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="8" t="s">
         <v>54</v>
       </c>
@@ -2454,7 +2457,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="8" t="s">
         <v>89</v>
       </c>
@@ -2527,7 +2530,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="8" t="s">
         <v>88</v>
       </c>
@@ -2596,7 +2599,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="8" t="s">
         <v>94</v>
       </c>
@@ -2667,7 +2670,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="8" t="s">
         <v>94</v>
       </c>
@@ -2738,7 +2741,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="8" t="s">
         <v>91</v>
       </c>
@@ -2810,7 +2813,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="8" t="s">
         <v>91</v>
       </c>
@@ -2880,7 +2883,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="8" t="s">
         <v>101</v>
       </c>
@@ -2953,7 +2956,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -2975,92 +2978,92 @@
       <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
-      <c r="B16" s="52" t="s">
+      <c r="A16" s="52"/>
+      <c r="B16" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46">
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37">
         <f>SUM(G2:G14)</f>
         <v>4801.9048451733333</v>
       </c>
-      <c r="H16" s="53">
+      <c r="H16" s="44">
         <f>SUM(H2:H14)</f>
         <v>4.8019048451733335</v>
       </c>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="46">
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="37">
         <f>SUM(P2:P14)</f>
         <v>3867.23101056</v>
       </c>
-      <c r="Q16" s="53">
+      <c r="Q16" s="44">
         <f>SUM(Q2:Q14)</f>
         <v>3.8672310105600003</v>
       </c>
-      <c r="R16" s="45"/>
-      <c r="S16" s="53">
+      <c r="R16" s="36"/>
+      <c r="S16" s="44">
         <f>SUM(S2:S14)</f>
         <v>0.93467383461333309</v>
       </c>
-      <c r="T16" s="55">
+      <c r="T16" s="46">
         <f>Q16/H16</f>
         <v>0.8053535284955039</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="50" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="G18" s="50" t="s">
+      <c r="G18" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="H18" s="51" t="s">
+      <c r="H18" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="K18" s="50" t="s">
+      <c r="K18" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="L18" s="50" t="s">
+      <c r="L18" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="M18" s="50" t="s">
+      <c r="M18" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="N18" s="50" t="s">
+      <c r="N18" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="O18" s="51" t="s">
+      <c r="O18" s="42" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="50" t="s">
         <v>106</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -3086,7 +3089,7 @@
         <f t="shared" ref="H19:H23" si="15">G19/1000</f>
         <v>0</v>
       </c>
-      <c r="J19" s="32"/>
+      <c r="J19" s="51"/>
       <c r="K19" s="8" t="s">
         <v>110</v>
       </c>
@@ -3107,7 +3110,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="A20" s="51"/>
       <c r="B20" s="8" t="s">
         <v>54</v>
       </c>
@@ -3133,7 +3136,7 @@
         <f t="shared" si="15"/>
         <v>4.4400000000000004E-3</v>
       </c>
-      <c r="J20" s="32"/>
+      <c r="J20" s="51"/>
       <c r="K20" s="8" t="s">
         <v>86</v>
       </c>
@@ -3155,7 +3158,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="8" t="s">
         <v>94</v>
       </c>
@@ -3180,7 +3183,7 @@
         <f t="shared" si="15"/>
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="J21" s="32"/>
+      <c r="J21" s="51"/>
       <c r="K21" s="8" t="s">
         <v>101</v>
       </c>
@@ -3202,7 +3205,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="8" t="s">
         <v>86</v>
       </c>
@@ -3227,7 +3230,7 @@
         <f t="shared" si="15"/>
         <v>3.3E-3</v>
       </c>
-      <c r="J22" s="32"/>
+      <c r="J22" s="51"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="19"/>
@@ -3235,7 +3238,7 @@
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="8" t="s">
         <v>96</v>
       </c>
@@ -3259,23 +3262,23 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J23" s="33"/>
+      <c r="J23" s="52"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="45" t="s">
+      <c r="M23" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="46">
+      <c r="N23" s="37">
         <f>SUM(N19:N21)</f>
         <v>4813.3448451733339</v>
       </c>
-      <c r="O23" s="47">
+      <c r="O23" s="38">
         <f>SUM(O19:O21)</f>
         <v>4.8133448451733338</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -3288,19 +3291,19 @@
       <c r="O24" s="5"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="33"/>
-      <c r="B25" s="52" t="s">
+      <c r="A25" s="52"/>
+      <c r="B25" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="54">
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="45">
         <f>SUM(G19:G23)</f>
         <v>11.440000000000001</v>
       </c>
-      <c r="H25" s="47">
+      <c r="H25" s="38">
         <f>SUM(H19:H23)</f>
         <v>1.1440000000000002E-2</v>
       </c>
@@ -3314,40 +3317,40 @@
       <c r="O26" s="5"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
       <c r="J27" s="2"/>
       <c r="M27" s="4"/>
       <c r="N27" s="6"/>
       <c r="O27" s="5"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
       <c r="J28" s="2"/>
       <c r="M28" s="7"/>
       <c r="N28" s="4"/>
       <c r="O28" s="5"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
       <c r="J29" s="2"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
@@ -3368,116 +3371,116 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B29:E29"/>
     <mergeCell ref="J18:J23"/>
     <mergeCell ref="A1:A16"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
   </mergeCells>
   <conditionalFormatting sqref="O2:O14">
-    <cfRule type="cellIs" dxfId="61" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="24" operator="lessThan">
       <formula>0.8*$I2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="52" priority="25" operator="between">
       <formula>$I2*0.8</formula>
       <formula>$I2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="28">
+    <cfRule type="expression" dxfId="51" priority="28">
       <formula>$O2&gt;$I2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E14">
-    <cfRule type="cellIs" dxfId="58" priority="21" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="50" priority="21" stopIfTrue="1" operator="between">
       <formula>$C2</formula>
       <formula>$D2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="22" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="23">
+    <cfRule type="expression" dxfId="48" priority="23">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N14">
-    <cfRule type="cellIs" dxfId="55" priority="19" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="47" priority="19" stopIfTrue="1" operator="between">
       <formula>$L2</formula>
       <formula>$M2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="20">
+    <cfRule type="expression" dxfId="46" priority="20">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S14">
-    <cfRule type="cellIs" dxfId="53" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T14 T16">
-    <cfRule type="cellIs" dxfId="52" priority="16" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="16" operator="greaterThanOrEqual">
       <formula>50%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="17" operator="lessThan">
       <formula>50%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="50" priority="13" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="13" stopIfTrue="1" operator="between">
       <formula>$C19</formula>
       <formula>"$D2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="14" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="15">
+    <cfRule type="expression" dxfId="40" priority="15">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="47" priority="10" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="10" stopIfTrue="1" operator="between">
       <formula>$C20</formula>
       <formula>"$D2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="11" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="12">
+    <cfRule type="expression" dxfId="37" priority="12">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="44" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="7" stopIfTrue="1" operator="between">
       <formula>$C21</formula>
       <formula>"$D2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="8" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="9">
+    <cfRule type="expression" dxfId="34" priority="9">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="41" priority="4" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="4" stopIfTrue="1" operator="between">
       <formula>$C22</formula>
       <formula>"$D2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="5" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="6">
+    <cfRule type="expression" dxfId="31" priority="6">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="38" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="between">
       <formula>$C23</formula>
       <formula>"$D2"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="2" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="3">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3509,28 +3512,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="40" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="28" t="s">
         <v>113</v>
       </c>
       <c r="C2" s="8">
@@ -3549,7 +3552,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3557,20 +3560,20 @@
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="45" cm="1">
+      <c r="D4" s="36" cm="1">
         <f t="array" ref="D4">Table5[Current (mA)]</f>
         <v>195</v>
       </c>
-      <c r="E4" s="46" cm="1">
+      <c r="E4" s="37" cm="1">
         <f t="array" ref="E4">Table5[Power (mW)]</f>
         <v>643.5</v>
       </c>
-      <c r="F4" s="47" cm="1">
+      <c r="F4" s="38" cm="1">
         <f t="array" ref="F4">Table5[Power (W)]</f>
         <v>0.64349999999999996</v>
       </c>
@@ -3591,8 +3594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE18E8FD-9EAF-459F-839D-AF6883546977}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3615,7 +3618,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="50" t="s">
         <v>68</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -3633,7 +3636,7 @@
       <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="50" t="s">
         <v>23</v>
       </c>
       <c r="I1" s="14" t="s">
@@ -3662,7 +3665,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
+      <c r="A2" s="51"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -3680,7 +3683,7 @@
         <f>E2/1000</f>
         <v>0.61250000000000004</v>
       </c>
-      <c r="H2" s="32"/>
+      <c r="H2" s="51"/>
       <c r="I2" s="8" t="s">
         <v>16</v>
       </c>
@@ -3711,7 +3714,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
@@ -3729,7 +3732,7 @@
         <f t="shared" ref="F3:F5" si="2">E3/1000</f>
         <v>1</v>
       </c>
-      <c r="H3" s="32"/>
+      <c r="H3" s="51"/>
       <c r="I3" s="8" t="s">
         <v>17</v>
       </c>
@@ -3760,7 +3763,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
@@ -3778,7 +3781,7 @@
         <f t="shared" si="2"/>
         <v>0.27</v>
       </c>
-      <c r="H4" s="32"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="8" t="s">
         <v>18</v>
       </c>
@@ -3809,7 +3812,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="8" t="s">
         <v>45</v>
       </c>
@@ -3828,7 +3831,7 @@
         <f t="shared" si="2"/>
         <v>0.54</v>
       </c>
-      <c r="H5" s="32"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="8" t="s">
         <v>19</v>
       </c>
@@ -3859,7 +3862,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
@@ -3877,7 +3880,7 @@
         <f t="shared" ref="F6:F13" si="6">E6/1000</f>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H6" s="32"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="8" t="s">
         <v>24</v>
       </c>
@@ -3908,7 +3911,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3926,7 +3929,7 @@
         <f t="shared" si="6"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="8" t="s">
         <v>20</v>
       </c>
@@ -3957,7 +3960,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
@@ -3975,7 +3978,7 @@
         <f t="shared" si="6"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H8" s="32"/>
+      <c r="H8" s="51"/>
       <c r="I8" s="8" t="s">
         <v>21</v>
       </c>
@@ -4006,7 +4009,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
@@ -4024,7 +4027,7 @@
         <f t="shared" si="6"/>
         <v>1.8E-3</v>
       </c>
-      <c r="H9" s="32"/>
+      <c r="H9" s="51"/>
       <c r="I9" s="8" t="s">
         <v>22</v>
       </c>
@@ -4055,7 +4058,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
@@ -4073,7 +4076,7 @@
         <f t="shared" si="6"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H10" s="32"/>
+      <c r="H10" s="51"/>
       <c r="I10" s="8" t="s">
         <v>25</v>
       </c>
@@ -4104,7 +4107,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
@@ -4122,7 +4125,7 @@
         <f t="shared" si="6"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H11" s="32"/>
+      <c r="H11" s="51"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -4133,7 +4136,7 @@
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
@@ -4151,7 +4154,7 @@
         <f t="shared" si="6"/>
         <v>0.27</v>
       </c>
-      <c r="H12" s="33"/>
+      <c r="H12" s="52"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="24" t="s">
@@ -4179,7 +4182,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="8" t="s">
         <v>60</v>
       </c>
@@ -4202,7 +4205,7 @@
       <c r="P13" s="3"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="8" t="s">
         <v>52</v>
       </c>
@@ -4224,7 +4227,7 @@
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="8" t="s">
         <v>51</v>
       </c>
@@ -4246,8 +4249,8 @@
       <c r="H15" s="1"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="51"/>
       <c r="B16" s="8" t="s">
         <v>48</v>
       </c>
@@ -4266,7 +4269,7 @@
         <f>E16/1000</f>
         <v>0.30960601056000003</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="55" t="s">
         <v>48</v>
       </c>
       <c r="I16" s="14" t="s">
@@ -4295,13 +4298,13 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
-      <c r="H17" s="32"/>
+      <c r="H17" s="56"/>
       <c r="I17" s="8" t="s">
         <v>28</v>
       </c>
@@ -4331,7 +4334,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="24" t="s">
@@ -4345,7 +4348,7 @@
         <f>SUM(F2:F16)</f>
         <v>3.2190810105600005</v>
       </c>
-      <c r="H18" s="32"/>
+      <c r="H18" s="56"/>
       <c r="I18" s="8" t="s">
         <v>29</v>
       </c>
@@ -4375,7 +4378,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H19" s="32"/>
+      <c r="H19" s="56"/>
       <c r="I19" s="8" t="s">
         <v>30</v>
       </c>
@@ -4405,7 +4408,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="50" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -4423,7 +4426,7 @@
       <c r="F20" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="32"/>
+      <c r="H20" s="56"/>
       <c r="I20" s="8" t="s">
         <v>31</v>
       </c>
@@ -4453,7 +4456,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="8" t="s">
         <v>2</v>
       </c>
@@ -4473,7 +4476,7 @@
         <f>E21/1000</f>
         <v>0.61250000000000004</v>
       </c>
-      <c r="H21" s="32"/>
+      <c r="H21" s="56"/>
       <c r="I21" s="8" t="s">
         <v>32</v>
       </c>
@@ -4503,7 +4506,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="8" t="s">
         <v>7</v>
       </c>
@@ -4523,7 +4526,7 @@
         <f t="shared" ref="F22:F29" si="13">E22/1000</f>
         <v>1</v>
       </c>
-      <c r="H22" s="32"/>
+      <c r="H22" s="56"/>
       <c r="I22" s="8" t="s">
         <v>33</v>
       </c>
@@ -4553,7 +4556,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="8" t="s">
         <v>67</v>
       </c>
@@ -4573,7 +4576,7 @@
         <f t="shared" si="13"/>
         <v>1.1088</v>
       </c>
-      <c r="H23" s="32"/>
+      <c r="H23" s="56"/>
       <c r="I23" s="8" t="s">
         <v>34</v>
       </c>
@@ -4603,7 +4606,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="8" t="s">
         <v>52</v>
       </c>
@@ -4623,7 +4626,7 @@
         <f t="shared" si="13"/>
         <v>0.17549999999999999</v>
       </c>
-      <c r="H24" s="32"/>
+      <c r="H24" s="56"/>
       <c r="I24" s="8" t="s">
         <v>35</v>
       </c>
@@ -4653,7 +4656,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="8" t="s">
         <v>51</v>
       </c>
@@ -4673,7 +4676,7 @@
         <f t="shared" si="13"/>
         <v>6.7500000000000004E-4</v>
       </c>
-      <c r="H25" s="32"/>
+      <c r="H25" s="56"/>
       <c r="I25" s="8" t="s">
         <v>36</v>
       </c>
@@ -4703,7 +4706,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="8" t="s">
         <v>11</v>
       </c>
@@ -4723,7 +4726,7 @@
         <f t="shared" si="13"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H26" s="32"/>
+      <c r="H26" s="56"/>
       <c r="I26" s="8" t="s">
         <v>37</v>
       </c>
@@ -4753,7 +4756,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="A27" s="51"/>
       <c r="B27" s="8" t="s">
         <v>66</v>
       </c>
@@ -4772,7 +4775,7 @@
         <f t="shared" si="13"/>
         <v>1.6988399999999997E-2</v>
       </c>
-      <c r="H27" s="32"/>
+      <c r="H27" s="56"/>
       <c r="I27" s="8" t="s">
         <v>38</v>
       </c>
@@ -4802,7 +4805,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="8" t="s">
         <v>65</v>
       </c>
@@ -4822,7 +4825,7 @@
         <f t="shared" si="13"/>
         <v>1.9601999999999998E-2</v>
       </c>
-      <c r="H28" s="32"/>
+      <c r="H28" s="56"/>
       <c r="I28" s="8" t="s">
         <v>39</v>
       </c>
@@ -4852,7 +4855,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="8" t="s">
         <v>9</v>
       </c>
@@ -4872,7 +4875,7 @@
         <f t="shared" si="13"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H29" s="32"/>
+      <c r="H29" s="56"/>
       <c r="I29" s="8" t="s">
         <v>40</v>
       </c>
@@ -4902,7 +4905,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
+      <c r="A30" s="51"/>
       <c r="B30" s="8" t="s">
         <v>61</v>
       </c>
@@ -4922,7 +4925,7 @@
         <f>E30/1000</f>
         <v>0.27301561056000001</v>
       </c>
-      <c r="H30" s="32"/>
+      <c r="H30" s="56"/>
       <c r="I30" s="8" t="s">
         <v>41</v>
       </c>
@@ -4952,13 +4955,13 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+      <c r="A31" s="51"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="9"/>
-      <c r="H31" s="26"/>
+      <c r="H31" s="56"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -4969,7 +4972,7 @@
       <c r="P31" s="9"/>
     </row>
     <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="33"/>
+      <c r="A32" s="52"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="24" t="s">
@@ -4983,7 +4986,7 @@
         <f>SUM(F21:F30)</f>
         <v>3.2190810105600001</v>
       </c>
-      <c r="H32" s="27"/>
+      <c r="H32" s="57"/>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
@@ -5010,16 +5013,17 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A20:A32"/>
-    <mergeCell ref="H16:H30"/>
     <mergeCell ref="H1:H12"/>
     <mergeCell ref="A1:A18"/>
+    <mergeCell ref="H16:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="4">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5029,7 +5033,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5044,10 +5048,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
@@ -5067,8 +5071,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="32" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="8">
@@ -5090,8 +5094,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="48"/>
+      <c r="B3" s="32" t="s">
         <v>55</v>
       </c>
       <c r="C3" s="8">
@@ -5114,8 +5118,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -5123,28 +5127,28 @@
       <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="36"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="34">
         <f>SUM(E2:E3)</f>
         <v>500.67500000000001</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="35">
         <f>SUM(F2:F3)</f>
         <v>0.50067499999999998</v>
       </c>
-      <c r="G5" s="37"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -5161,12 +5165,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="40" t="s">
+      <c r="A8" s="48"/>
+      <c r="B8" s="32" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="8">
-        <f t="shared" ref="C8:C9" si="0">C2</f>
+        <f t="shared" ref="C8" si="0">C2</f>
         <v>1.35</v>
       </c>
       <c r="D8" s="17">
@@ -5183,8 +5187,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="40" t="s">
+      <c r="A9" s="48"/>
+      <c r="B9" s="32" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="8">
@@ -5205,25 +5209,25 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="37">
         <f>SUM(E8:E9)</f>
         <v>1001.3499999999999</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="38">
         <f>SUM(F8:F9)</f>
         <v>1.00135</v>
       </c>

</xml_diff>